<commit_message>
add preprocessing, add features
added some preprocessing features to the preprocessing script, saving in separate columns

added some feature extraction to featureEngineer script.
</commit_message>
<xml_diff>
--- a/asapData/rawData/sampleEssayAI.xlsx
+++ b/asapData/rawData/sampleEssayAI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ssserver4\slredirect$\AS\birdipa2\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/asapData/rawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F2C621-136B-47C4-A146-94FC596A55AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{B4F2C621-136B-47C4-A146-94FC596A55AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{400F29E7-663B-B94E-834E-B4766E10C7CC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{DA9ED9DE-7E78-4324-A704-197D1D906248}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="10400" xr2:uid="{DA9ED9DE-7E78-4324-A704-197D1D906248}"/>
   </bookViews>
   <sheets>
     <sheet name="Essay Set 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Dear Editor,
 As the use of computers becomes more widespread, the debate over their impact on society intensifies. While some may argue that the growth in technology has only positive effects, I firmly believe that the increasing reliance on computers has detrimental effects on people and the world around us.
@@ -123,6 +123,12 @@
 In conclusion, while there may be some valid concerns about the effects of computers on society, the benefits far outweigh the drawbacks. We should embrace technology as a tool for personal and societal growth, and continue to explore its potential to improve our lives.
 Sincerely,
 [Your Name]</t>
+  </si>
+  <si>
+    <t>essay</t>
+  </si>
+  <si>
+    <t>essay_set</t>
   </si>
 </sst>
 </file>
@@ -158,9 +164,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,63 +480,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D188D3E-6413-4D6A-A395-9B071BF990CD}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="173.21875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="173.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>